<commit_message>
Completed first draft of part 3
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,25 +408,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -465,22 +447,40 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -762,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:V16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -776,42 +776,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="F2" s="28"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="4" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:22" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="44"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="46" t="s">
+      <c r="B5" s="38"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="46"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="48" t="s">
+      <c r="E5" s="50"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="48" t="s">
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="48" t="s">
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="R5" s="46"/>
-      <c r="S5" s="46"/>
-      <c r="T5" s="46"/>
-      <c r="U5" s="47"/>
+      <c r="R5" s="50"/>
+      <c r="S5" s="50"/>
+      <c r="T5" s="50"/>
+      <c r="U5" s="51"/>
     </row>
-    <row r="6" spans="2:22" s="2" customFormat="1" ht="141" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="45"/>
-      <c r="C6" s="35"/>
+    <row r="6" spans="2:22" s="2" customFormat="1" ht="144" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="39"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="23" t="s">
         <v>15</v>
       </c>
@@ -884,49 +884,49 @@
       <c r="F7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="40">
         <v>43</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="41">
         <v>56</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="41">
         <v>180</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="41">
         <v>6</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="42">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="40">
         <v>3343</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="41">
         <v>4609</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="41">
         <v>30509</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="41">
         <v>9</v>
       </c>
-      <c r="P7" s="8">
+      <c r="P7" s="42">
         <v>12.569000000000001</v>
       </c>
       <c r="Q7" s="40">
         <v>14663</v>
       </c>
-      <c r="R7" s="36">
+      <c r="R7" s="41">
         <v>18098</v>
       </c>
-      <c r="S7" s="36">
+      <c r="S7" s="41">
         <v>129631</v>
       </c>
-      <c r="T7" s="6">
+      <c r="T7" s="41">
         <v>12</v>
       </c>
-      <c r="U7" s="41">
+      <c r="U7" s="42">
         <v>92.650999999999996</v>
       </c>
     </row>
@@ -961,20 +961,20 @@
       <c r="K8" s="13">
         <v>0.89200000000000002</v>
       </c>
-      <c r="L8" s="25" t="s">
+      <c r="L8" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="25" t="s">
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="R8" s="26"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="26"/>
-      <c r="U8" s="27"/>
+      <c r="R8" s="44"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="44"/>
+      <c r="U8" s="45"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B9" s="4">
@@ -1001,7 +1001,7 @@
       <c r="I9" s="6">
         <v>84</v>
       </c>
-      <c r="J9" s="37">
+      <c r="J9" s="31">
         <v>20</v>
       </c>
       <c r="K9" s="8">
@@ -1063,26 +1063,26 @@
       <c r="I10" s="11">
         <v>414</v>
       </c>
-      <c r="J10" s="36">
+      <c r="J10" s="30">
         <v>50</v>
       </c>
       <c r="K10" s="13">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="L10" s="25" t="s">
+      <c r="L10" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="25" t="s">
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="45"/>
+      <c r="Q10" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="R10" s="26"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="26"/>
-      <c r="U10" s="27"/>
+      <c r="R10" s="44"/>
+      <c r="S10" s="44"/>
+      <c r="T10" s="44"/>
+      <c r="U10" s="45"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B11" s="4">
@@ -1091,58 +1091,58 @@
       <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="32">
+      <c r="D11" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="26">
         <v>55</v>
       </c>
-      <c r="H11" s="33">
+      <c r="H11" s="27">
         <v>57</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="27">
         <v>224</v>
       </c>
-      <c r="J11" s="33">
+      <c r="J11" s="27">
         <v>6</v>
       </c>
-      <c r="K11" s="34">
+      <c r="K11" s="28">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="L11" s="38">
+      <c r="L11" s="32">
         <v>4853</v>
       </c>
-      <c r="M11" s="39">
+      <c r="M11" s="33">
         <v>4855</v>
       </c>
-      <c r="N11" s="39">
+      <c r="N11" s="33">
         <v>44041</v>
       </c>
-      <c r="O11" s="33">
+      <c r="O11" s="27">
         <v>9</v>
       </c>
-      <c r="P11" s="34">
+      <c r="P11" s="28">
         <v>11.12</v>
       </c>
-      <c r="Q11" s="38">
+      <c r="Q11" s="32">
         <v>18162</v>
       </c>
-      <c r="R11" s="39">
+      <c r="R11" s="33">
         <v>18164</v>
       </c>
-      <c r="S11" s="39">
+      <c r="S11" s="33">
         <v>159128</v>
       </c>
-      <c r="T11" s="33">
+      <c r="T11" s="27">
         <v>12</v>
       </c>
-      <c r="U11" s="42">
+      <c r="U11" s="36">
         <v>49.595999999999997</v>
       </c>
     </row>
@@ -1177,20 +1177,20 @@
       <c r="K12" s="13">
         <v>2.9780000000000002</v>
       </c>
-      <c r="L12" s="25" t="s">
+      <c r="L12" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="25" t="s">
+      <c r="M12" s="44"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="R12" s="26"/>
-      <c r="S12" s="26"/>
-      <c r="T12" s="26"/>
-      <c r="U12" s="27"/>
+      <c r="R12" s="44"/>
+      <c r="S12" s="44"/>
+      <c r="T12" s="44"/>
+      <c r="U12" s="45"/>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B13" s="4">
@@ -1208,19 +1208,19 @@
       <c r="F13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="49">
+      <c r="G13" s="40">
         <v>7</v>
       </c>
-      <c r="H13" s="50">
+      <c r="H13" s="41">
         <v>9</v>
       </c>
-      <c r="I13" s="50">
+      <c r="I13" s="41">
         <v>28</v>
       </c>
-      <c r="J13" s="50">
+      <c r="J13" s="41">
         <v>6</v>
       </c>
-      <c r="K13" s="51">
+      <c r="K13" s="42">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="L13" s="7">
@@ -1285,13 +1285,13 @@
       <c r="K14" s="13">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="L14" s="40">
+      <c r="L14" s="34">
         <v>4853</v>
       </c>
-      <c r="M14" s="36">
+      <c r="M14" s="30">
         <v>4855</v>
       </c>
-      <c r="N14" s="36">
+      <c r="N14" s="30">
         <v>44041</v>
       </c>
       <c r="O14" s="11">
@@ -1300,19 +1300,19 @@
       <c r="P14" s="13">
         <v>12.19</v>
       </c>
-      <c r="Q14" s="40">
+      <c r="Q14" s="34">
         <v>18162</v>
       </c>
-      <c r="R14" s="36">
+      <c r="R14" s="30">
         <v>18164</v>
       </c>
-      <c r="S14" s="36">
+      <c r="S14" s="30">
         <v>159128</v>
       </c>
       <c r="T14" s="11">
         <v>12</v>
       </c>
-      <c r="U14" s="41">
+      <c r="U14" s="35">
         <v>53.820999999999998</v>
       </c>
     </row>
@@ -1332,49 +1332,49 @@
       <c r="F15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="40">
         <v>41</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="41">
         <v>43</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="41">
         <v>170</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="41">
         <v>6</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15" s="42">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="L15" s="7">
+      <c r="L15" s="40">
         <v>1450</v>
       </c>
-      <c r="M15" s="6">
+      <c r="M15" s="41">
         <v>1452</v>
       </c>
-      <c r="N15" s="6">
+      <c r="N15" s="41">
         <v>13303</v>
       </c>
-      <c r="O15" s="6">
+      <c r="O15" s="41">
         <v>9</v>
       </c>
-      <c r="P15" s="8">
+      <c r="P15" s="42">
         <v>4.452</v>
       </c>
-      <c r="Q15" s="7">
+      <c r="Q15" s="40">
         <v>5038</v>
       </c>
-      <c r="R15" s="6">
+      <c r="R15" s="41">
         <v>5040</v>
       </c>
-      <c r="S15" s="6">
+      <c r="S15" s="41">
         <v>44924</v>
       </c>
-      <c r="T15" s="6">
+      <c r="T15" s="41">
         <v>12</v>
       </c>
-      <c r="U15" s="8">
+      <c r="U15" s="42">
         <v>17.321000000000002</v>
       </c>
     </row>
@@ -1409,23 +1409,28 @@
       <c r="K16" s="18">
         <v>1.147</v>
       </c>
-      <c r="L16" s="29" t="s">
+      <c r="L16" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="31"/>
-      <c r="Q16" s="29" t="s">
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="48"/>
+      <c r="Q16" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="R16" s="30"/>
-      <c r="S16" s="30"/>
-      <c r="T16" s="30"/>
-      <c r="U16" s="31"/>
+      <c r="R16" s="47"/>
+      <c r="S16" s="47"/>
+      <c r="T16" s="47"/>
+      <c r="U16" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="L8:P8"/>
+    <mergeCell ref="L10:P10"/>
+    <mergeCell ref="Q8:U8"/>
+    <mergeCell ref="Q10:U10"/>
     <mergeCell ref="L12:P12"/>
     <mergeCell ref="L16:P16"/>
     <mergeCell ref="Q12:U12"/>
@@ -1433,11 +1438,6 @@
     <mergeCell ref="G5:K5"/>
     <mergeCell ref="L5:P5"/>
     <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="L8:P8"/>
-    <mergeCell ref="L10:P10"/>
-    <mergeCell ref="Q8:U8"/>
-    <mergeCell ref="Q10:U10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>